<commit_message>
Assessment summary page fixes
</commit_message>
<xml_diff>
--- a/src/wise/msfd/data/MSmarinewaters_MRUs_statistics_2021-05-03.xlsx
+++ b/src/wise/msfd/data/MSmarinewaters_MRUs_statistics_2021-05-03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MS source files" sheetId="1" state="visible" r:id="rId2"/>
@@ -6072,7 +6072,7 @@
       <selection pane="bottomRight" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16"/>
@@ -7563,15 +7563,15 @@
   </sheetPr>
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="I39" activeCellId="0" sqref="I39"/>
+      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="K35" activeCellId="0" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="87" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="87" width="12.28"/>
@@ -10366,11 +10366,11 @@
   </sheetPr>
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.77"/>
@@ -10378,8 +10378,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="7" style="18" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="18" width="9.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="18" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="18" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="18" width="16.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="11" style="18" width="8.7"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="1" width="8.7"/>
   </cols>

</xml_diff>

<commit_message>
Updated marine waters data
</commit_message>
<xml_diff>
--- a/src/wise/msfd/data/MSmarinewaters_MRUs_statistics_2021-05-03.xlsx
+++ b/src/wise/msfd/data/MSmarinewaters_MRUs_statistics_2021-05-03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="MS source files" sheetId="1" state="visible" r:id="rId2"/>
@@ -6064,7 +6064,7 @@
   </sheetPr>
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -7547,7 +7547,7 @@
     <hyperlink ref="W26" r:id="rId70" display="http://cdr.eionet.europa.eu/gb/eu/msfd8910/msfd4geo/envuo1uhw"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -7563,11 +7563,11 @@
   </sheetPr>
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
       <selection pane="bottomRight" activeCell="K35" activeCellId="0" sqref="K35"/>
     </sheetView>
   </sheetViews>
@@ -10120,7 +10120,7 @@
     <mergeCell ref="B37:B40"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -10350,7 +10350,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -11566,7 +11566,7 @@
     <mergeCell ref="J33:J35"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -11582,7 +11582,7 @@
   </sheetPr>
   <dimension ref="A1:K860"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A572" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="H611" activeCellId="0" sqref="H611"/>
@@ -37437,7 +37437,7 @@
     <hyperlink ref="F841" r:id="rId822" display="http://cdr.eionet.europa.eu/gb/eu/msfd8910/msfd4geo/envuo1uhw/ANSUK_MSFD4Geo_20130109.xml/manage_document"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -37968,7 +37968,7 @@
     <mergeCell ref="A26:F27"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>